<commit_message>
Fixed position errors to csvParser.m
</commit_message>
<xml_diff>
--- a/Automation/Parsing/InterpolatedResults.xlsx
+++ b/Automation/Parsing/InterpolatedResults.xlsx
@@ -15,43 +15,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>NodeNumbers</t>
+    <t>CutLocation</t>
   </si>
   <si>
-    <t>XLocations_inches_</t>
+    <t>X Locations (inches)</t>
   </si>
   <si>
-    <t>YLocations_inches_</t>
+    <t>Y Locations (inches)</t>
   </si>
   <si>
-    <t>ZLocations_inches_</t>
+    <t>Z Locations (inches)</t>
   </si>
   <si>
-    <t>EquivalentElasticStrains_in_in_</t>
+    <t>Equivalent Elastic Strains (in/in)</t>
   </si>
   <si>
-    <t>EquivalentStress_psi_</t>
+    <t>Equivalent Stress (psi)</t>
   </si>
   <si>
-    <t>MaxPrincipalElasticStrain_in_in_</t>
+    <t>Max Principal Elastic Strain (in/in)</t>
   </si>
   <si>
-    <t>MaxPrincipalStress_psi_</t>
+    <t>Max Principal Stress (psi)</t>
   </si>
   <si>
-    <t>MiddlePrincipalElasticStrain_in_in_</t>
+    <t>Middle Principal Elastic Strain (in/in)</t>
   </si>
   <si>
-    <t>MiddlePrincipalStress_psi_</t>
+    <t>Middle Principal Stress (psi)</t>
   </si>
   <si>
-    <t>MinPrincipalElasticStrain_in_in_</t>
+    <t>Min Principal Elastic Strain (in/in)</t>
   </si>
   <si>
-    <t>MinPrincipalStress_psi_</t>
+    <t>Min Principal Stress (psi)</t>
   </si>
   <si>
-    <t>TotalDeformation_in_</t>
+    <t>Total Deformation (in)</t>
   </si>
 </sst>
 </file>
@@ -100,18 +100,18 @@
   <dimension ref="A1:M103"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.93359375" customWidth="true"/>
+    <col min="1" max="1" width="11.046875" customWidth="true"/>
     <col min="2" max="2" width="17.15625" customWidth="true"/>
     <col min="3" max="3" width="17.15625" customWidth="true"/>
     <col min="4" max="4" width="17.046875" customWidth="true"/>
-    <col min="5" max="5" width="26.15625" customWidth="true"/>
+    <col min="5" max="5" width="26.37890625" customWidth="true"/>
     <col min="6" max="6" width="18.6015625" customWidth="true"/>
-    <col min="7" max="7" width="27.37890625" customWidth="true"/>
-    <col min="8" max="8" width="20.6015625" customWidth="true"/>
-    <col min="9" max="9" width="29.37890625" customWidth="true"/>
-    <col min="10" max="10" width="22.6015625" customWidth="true"/>
-    <col min="11" max="11" width="26.93359375" customWidth="true"/>
-    <col min="12" max="12" width="20.15625" customWidth="true"/>
+    <col min="7" max="7" width="28.046875" customWidth="true"/>
+    <col min="8" max="8" width="21.046875" customWidth="true"/>
+    <col min="9" max="9" width="30.046875" customWidth="true"/>
+    <col min="10" max="10" width="23.046875" customWidth="true"/>
+    <col min="11" max="11" width="27.6015625" customWidth="true"/>
+    <col min="12" max="12" width="20.6015625" customWidth="true"/>
     <col min="13" max="13" width="19.26953125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -158,7 +158,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -167,7 +167,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>0.063473553980008382</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0">
         <v>0.0005756625396869606</v>
@@ -199,7 +199,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>3.02</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
@@ -208,7 +208,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="0">
-        <v>0.063450671172299369</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0">
         <v>0.00058005139520436711</v>
@@ -240,7 +240,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>3.04</v>
       </c>
       <c r="B4" s="0">
         <v>1</v>
@@ -249,7 +249,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="0">
-        <v>0.063407645361963444</v>
+        <v>1</v>
       </c>
       <c r="E4" s="0">
         <v>0.00058428965874406406</v>
@@ -281,7 +281,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>1</v>
+        <v>3.0600000000000001</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
@@ -290,7 +290,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="0">
-        <v>0.087478496730551469</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0">
         <v>0.0005989520417291126</v>
@@ -322,7 +322,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>1</v>
+        <v>3.0800000000000001</v>
       </c>
       <c r="B6" s="0">
         <v>1</v>
@@ -331,7 +331,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>0.075492997754250057</v>
+        <v>1</v>
       </c>
       <c r="E6" s="0">
         <v>0.00055690867299390437</v>
@@ -363,7 +363,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>1</v>
+        <v>3.1000000000000001</v>
       </c>
       <c r="B7" s="0">
         <v>1</v>
@@ -372,7 +372,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="0">
-        <v>0.075432398987274316</v>
+        <v>1</v>
       </c>
       <c r="E7" s="0">
         <v>0.00055721586782391983</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>1</v>
+        <v>3.1200000000000001</v>
       </c>
       <c r="B8" s="0">
         <v>1</v>
@@ -413,7 +413,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="0">
-        <v>0.087827884806605971</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0">
         <v>0.00056907900426554116</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1</v>
+        <v>3.1400000000000001</v>
       </c>
       <c r="B9" s="0">
         <v>1</v>
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="0">
-        <v>0.075307296269255336</v>
+        <v>1</v>
       </c>
       <c r="E9" s="0">
         <v>0.00054519877963217142</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>1</v>
+        <v>3.1600000000000001</v>
       </c>
       <c r="B10" s="0">
         <v>1</v>
@@ -495,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="0">
-        <v>0.052207345653740474</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0">
         <v>0.00052769567646680489</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>1</v>
+        <v>3.1800000000000002</v>
       </c>
       <c r="B11" s="0">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="0">
-        <v>0.052072969879214337</v>
+        <v>1</v>
       </c>
       <c r="E11" s="0">
         <v>0.00054576549001498879</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>1</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="B12" s="0">
         <v>1</v>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="0">
-        <v>0.052201651445535222</v>
+        <v>1</v>
       </c>
       <c r="E12" s="0">
         <v>0.00056404336701848913</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1</v>
+        <v>3.2200000000000002</v>
       </c>
       <c r="B13" s="0">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="0">
-        <v>0.052204751774990135</v>
+        <v>1</v>
       </c>
       <c r="E13" s="0">
         <v>0.00053189151300650256</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1</v>
+        <v>3.2400000000000002</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="0">
-        <v>0.052209604108309118</v>
+        <v>1</v>
       </c>
       <c r="E14" s="0">
         <v>0.0005712597315704306</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>1</v>
+        <v>3.2599999999999998</v>
       </c>
       <c r="B15" s="0">
         <v>1</v>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="0">
-        <v>0.052207080823518083</v>
+        <v>1</v>
       </c>
       <c r="E15" s="0">
         <v>0.00057066286439763864</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1</v>
+        <v>3.2799999999999998</v>
       </c>
       <c r="B16" s="0">
         <v>1</v>
@@ -741,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="0">
-        <v>0.087737794779260969</v>
+        <v>1</v>
       </c>
       <c r="E16" s="0">
         <v>0.00055443705305479002</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1</v>
+        <v>3.2999999999999998</v>
       </c>
       <c r="B17" s="0">
         <v>1</v>
@@ -782,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="0">
-        <v>0.087583234459745599</v>
+        <v>1</v>
       </c>
       <c r="E17" s="0">
         <v>0.00055739620299883664</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>1</v>
+        <v>3.3199999999999998</v>
       </c>
       <c r="B18" s="0">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="0">
-        <v>0.087753742535823812</v>
+        <v>1</v>
       </c>
       <c r="E18" s="0">
         <v>0.00055634330307684882</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1</v>
+        <v>3.3399999999999999</v>
       </c>
       <c r="B19" s="0">
         <v>1</v>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="0">
-        <v>0.087910127977886124</v>
+        <v>1</v>
       </c>
       <c r="E19" s="0">
         <v>0.00055169571800765566</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>1</v>
+        <v>3.3599999999999999</v>
       </c>
       <c r="B20" s="0">
         <v>1</v>
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="0">
-        <v>0.08772368352810922</v>
+        <v>1</v>
       </c>
       <c r="E20" s="0">
         <v>0.00054246295022222779</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1</v>
+        <v>3.3799999999999999</v>
       </c>
       <c r="B21" s="0">
         <v>1</v>
@@ -946,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="0">
-        <v>0.087772118818841102</v>
+        <v>1</v>
       </c>
       <c r="E21" s="0">
         <v>0.00054211267760353988</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>1</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="B22" s="0">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="0">
-        <v>0.075847568255467041</v>
+        <v>1</v>
       </c>
       <c r="E22" s="0">
         <v>0.00055502973495830652</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>1</v>
+        <v>3.4199999999999999</v>
       </c>
       <c r="B23" s="0">
         <v>1</v>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="0">
-        <v>0.087626973883777715</v>
+        <v>1</v>
       </c>
       <c r="E23" s="0">
         <v>0.00056161765368595816</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>1</v>
+        <v>3.4399999999999999</v>
       </c>
       <c r="B24" s="0">
         <v>1</v>
@@ -1069,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="0">
-        <v>0.087639870796661648</v>
+        <v>1</v>
       </c>
       <c r="E24" s="0">
         <v>0.00055417349717153531</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1</v>
+        <v>3.46</v>
       </c>
       <c r="B25" s="0">
         <v>1</v>
@@ -1110,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="0">
-        <v>0.087701904316929494</v>
+        <v>1</v>
       </c>
       <c r="E25" s="0">
         <v>0.00055863609788893464</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>1</v>
+        <v>3.48</v>
       </c>
       <c r="B26" s="0">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="0">
-        <v>0.087603234076879227</v>
+        <v>1</v>
       </c>
       <c r="E26" s="0">
         <v>0.00055547316416357175</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="B27" s="0">
         <v>1</v>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="0">
-        <v>0.087911206423059329</v>
+        <v>1</v>
       </c>
       <c r="E27" s="0">
         <v>0.00054080675925067471</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>1</v>
+        <v>3.52</v>
       </c>
       <c r="B28" s="0">
         <v>1</v>
@@ -1233,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="0">
-        <v>0.087839024424965301</v>
+        <v>1</v>
       </c>
       <c r="E28" s="0">
         <v>0.00054954595497795308</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>1</v>
+        <v>3.54</v>
       </c>
       <c r="B29" s="0">
         <v>1</v>
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="0">
-        <v>0.063255482543113362</v>
+        <v>1</v>
       </c>
       <c r="E29" s="0">
         <v>0.00055081094684283959</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>1</v>
+        <v>3.5600000000000001</v>
       </c>
       <c r="B30" s="0">
         <v>1</v>
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="0">
-        <v>0.063507747281295601</v>
+        <v>1</v>
       </c>
       <c r="E30" s="0">
         <v>0.00057599787629669099</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1</v>
+        <v>3.5800000000000001</v>
       </c>
       <c r="B31" s="0">
         <v>1</v>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="0">
-        <v>0.063270054617001109</v>
+        <v>1</v>
       </c>
       <c r="E31" s="0">
         <v>0.00057411485697270149</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="B32" s="0">
         <v>1</v>
@@ -1397,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="0">
-        <v>0.063242025957830059</v>
+        <v>1</v>
       </c>
       <c r="E32" s="0">
         <v>0.00056861341270959213</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1</v>
+        <v>3.6200000000000001</v>
       </c>
       <c r="B33" s="0">
         <v>1</v>
@@ -1438,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="0">
-        <v>0.063594199783344268</v>
+        <v>1</v>
       </c>
       <c r="E33" s="0">
         <v>0.00057542464381152335</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>1</v>
+        <v>3.6400000000000001</v>
       </c>
       <c r="B34" s="0">
         <v>1</v>
@@ -1479,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="0">
-        <v>0.087991519008715796</v>
+        <v>1</v>
       </c>
       <c r="E34" s="0">
         <v>0.00053318424021597908</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1</v>
+        <v>3.6600000000000001</v>
       </c>
       <c r="B35" s="0">
         <v>1</v>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="0">
-        <v>0.088067495475574992</v>
+        <v>1</v>
       </c>
       <c r="E35" s="0">
         <v>0.00054657154894115082</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>1</v>
+        <v>3.6800000000000002</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="0">
-        <v>0.088100575180972709</v>
+        <v>1</v>
       </c>
       <c r="E36" s="0">
         <v>0.0005597930633095998</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>1</v>
+        <v>3.7000000000000002</v>
       </c>
       <c r="B37" s="0">
         <v>1</v>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="0">
-        <v>0.087556366409849734</v>
+        <v>1</v>
       </c>
       <c r="E37" s="0">
         <v>0.00059628344122467905</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1</v>
+        <v>3.7200000000000002</v>
       </c>
       <c r="B38" s="0">
         <v>1</v>
@@ -1643,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="0">
-        <v>0.087558165864310408</v>
+        <v>1</v>
       </c>
       <c r="E38" s="0">
         <v>0.00059612075067610678</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>1</v>
+        <v>3.7400000000000002</v>
       </c>
       <c r="B39" s="0">
         <v>1</v>
@@ -1684,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="0">
-        <v>0.087548415642839314</v>
+        <v>1</v>
       </c>
       <c r="E39" s="0">
         <v>0.0005964220617304545</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>1</v>
+        <v>3.7599999999999998</v>
       </c>
       <c r="B40" s="0">
         <v>1</v>
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="0">
-        <v>0.087526127242807256</v>
+        <v>1</v>
       </c>
       <c r="E40" s="0">
         <v>0.000596763244223714</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1</v>
+        <v>3.7799999999999998</v>
       </c>
       <c r="B41" s="0">
         <v>1</v>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="0">
-        <v>0.087515265479676835</v>
+        <v>1</v>
       </c>
       <c r="E41" s="0">
         <v>0.00059906575679243674</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>1</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="B42" s="0">
         <v>1</v>
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="0">
-        <v>0.08750630263808104</v>
+        <v>1</v>
       </c>
       <c r="E42" s="0">
         <v>0.00059876340415675557</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>1</v>
+        <v>3.8199999999999998</v>
       </c>
       <c r="B43" s="0">
         <v>1</v>
@@ -1848,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="0">
-        <v>0.087476774164667356</v>
+        <v>1</v>
       </c>
       <c r="E43" s="0">
         <v>0.00059450508119448717</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1</v>
+        <v>3.8399999999999999</v>
       </c>
       <c r="B44" s="0">
         <v>1</v>
@@ -1889,7 +1889,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="0">
-        <v>0.087486293767285631</v>
+        <v>1</v>
       </c>
       <c r="E44" s="0">
         <v>0.00059921039058143403</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>1</v>
+        <v>3.8599999999999999</v>
       </c>
       <c r="B45" s="0">
         <v>1</v>
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="0">
-        <v>0.087476118022980193</v>
+        <v>1</v>
       </c>
       <c r="E45" s="0">
         <v>0.0005993475396179834</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>1</v>
+        <v>3.8799999999999999</v>
       </c>
       <c r="B46" s="0">
         <v>1</v>
@@ -1971,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="0">
-        <v>0.087465820989092405</v>
+        <v>1</v>
       </c>
       <c r="E46" s="0">
         <v>0.00059947719909314221</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1</v>
+        <v>3.8999999999999999</v>
       </c>
       <c r="B47" s="0">
         <v>1</v>
@@ -2012,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="0">
-        <v>0.063790688239866306</v>
+        <v>1</v>
       </c>
       <c r="E47" s="0">
         <v>0.00061279487763102943</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>1</v>
+        <v>3.9199999999999999</v>
       </c>
       <c r="B48" s="0">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="0">
-        <v>0.087649854301962898</v>
+        <v>1</v>
       </c>
       <c r="E48" s="0">
         <v>0.00059052473192478514</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>1</v>
+        <v>3.9399999999999999</v>
       </c>
       <c r="B49" s="0">
         <v>1</v>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="0">
-        <v>0.087843221576513669</v>
+        <v>1</v>
       </c>
       <c r="E49" s="0">
         <v>0.0005934931105806532</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>1</v>
+        <v>3.96</v>
       </c>
       <c r="B50" s="0">
         <v>1</v>
@@ -2135,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="0">
-        <v>0.087628090912366688</v>
+        <v>1</v>
       </c>
       <c r="E50" s="0">
         <v>0.00058918573856565578</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>1</v>
+        <v>3.98</v>
       </c>
       <c r="B51" s="0">
         <v>1</v>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="0">
-        <v>0.08764560786974511</v>
+        <v>1</v>
       </c>
       <c r="E51" s="0">
         <v>0.00058724866890337199</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B52" s="0">
         <v>1</v>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="0">
-        <v>0.087398137810033333</v>
+        <v>1</v>
       </c>
       <c r="E52" s="0">
         <v>0.00060099301740426984</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>1</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="B53" s="0">
         <v>1</v>
@@ -2258,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="0">
-        <v>0.088069825780623889</v>
+        <v>1</v>
       </c>
       <c r="E53" s="0">
         <v>0.0001030660953552675</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>1</v>
+        <v>4.04</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="0">
-        <v>0.063473409807053766</v>
+        <v>1</v>
       </c>
       <c r="E54" s="0">
         <v>0.00010624344024900818</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>1</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="B55" s="0">
         <v>1</v>
@@ -2340,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="0">
-        <v>0.063389315931484239</v>
+        <v>1</v>
       </c>
       <c r="E55" s="0">
         <v>0.00010710026463787215</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>1</v>
+        <v>4.0800000000000001</v>
       </c>
       <c r="B56" s="0">
         <v>1</v>
@@ -2381,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="0">
-        <v>0.063389315931484239</v>
+        <v>1</v>
       </c>
       <c r="E56" s="0">
         <v>0.00010710026463787215</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B57" s="0">
         <v>1</v>
@@ -2422,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="0">
-        <v>0.063389820470469274</v>
+        <v>1</v>
       </c>
       <c r="E57" s="0">
         <v>0.00010703150170022132</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>1</v>
+        <v>4.1200000000000001</v>
       </c>
       <c r="B58" s="0">
         <v>1</v>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="0">
-        <v>0.063520156192761815</v>
+        <v>1</v>
       </c>
       <c r="E58" s="0">
         <v>0.00010648298472072697</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>1</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="B59" s="0">
         <v>1</v>
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="0">
-        <v>0.063403045025889976</v>
+        <v>1</v>
       </c>
       <c r="E59" s="0">
         <v>0.00010693714971542168</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>1</v>
+        <v>4.1600000000000001</v>
       </c>
       <c r="B60" s="0">
         <v>1</v>
@@ -2545,7 +2545,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="0">
-        <v>0.063511656422488696</v>
+        <v>1</v>
       </c>
       <c r="E60" s="0">
         <v>0.00010710791361047037</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>1</v>
+        <v>4.1799999999999997</v>
       </c>
       <c r="B61" s="0">
         <v>1</v>
@@ -2586,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="0">
-        <v>0.087492566225716481</v>
+        <v>1</v>
       </c>
       <c r="E61" s="0">
         <v>0.00010184567337204477</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>1</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="B62" s="0">
         <v>1</v>
@@ -2627,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="0">
-        <v>0.087497815437413778</v>
+        <v>1</v>
       </c>
       <c r="E62" s="0">
         <v>0.00010183982995638891</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>1</v>
+        <v>4.2199999999999998</v>
       </c>
       <c r="B63" s="0">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="0">
-        <v>0.075774348011447071</v>
+        <v>1</v>
       </c>
       <c r="E63" s="0">
         <v>0.00012835171448600385</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>1</v>
+        <v>4.2400000000000002</v>
       </c>
       <c r="B64" s="0">
         <v>1</v>
@@ -2709,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="0">
-        <v>0.075736461929464385</v>
+        <v>1</v>
       </c>
       <c r="E64" s="0">
         <v>0.00012824740433469426</v>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>1</v>
+        <v>4.2599999999999998</v>
       </c>
       <c r="B65" s="0">
         <v>1</v>
@@ -2750,7 +2750,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="0">
-        <v>0.075697984479959124</v>
+        <v>1</v>
       </c>
       <c r="E65" s="0">
         <v>0.00012759314116567389</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>1</v>
+        <v>4.2800000000000002</v>
       </c>
       <c r="B66" s="0">
         <v>1</v>
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="0">
-        <v>0.052230410211285438</v>
+        <v>1</v>
       </c>
       <c r="E66" s="0">
         <v>0.00013043058431538889</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>1</v>
+        <v>4.2999999999999998</v>
       </c>
       <c r="B67" s="0">
         <v>1</v>
@@ -2832,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="0">
-        <v>0.052228366085782171</v>
+        <v>1</v>
       </c>
       <c r="E67" s="0">
         <v>0.00012759310398543258</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>1</v>
+        <v>4.3200000000000003</v>
       </c>
       <c r="B68" s="0">
         <v>1</v>
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="0">
-        <v>0.052202581494260519</v>
+        <v>1</v>
       </c>
       <c r="E68" s="0">
         <v>0.00012965078229610288</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>1</v>
+        <v>4.3399999999999999</v>
       </c>
       <c r="B69" s="0">
         <v>1</v>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="0">
-        <v>0.075800735396907487</v>
+        <v>1</v>
       </c>
       <c r="E69" s="0">
         <v>0.00013612053344531921</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>1</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="B70" s="0">
         <v>1</v>
@@ -2955,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="0">
-        <v>0.075807025411943479</v>
+        <v>1</v>
       </c>
       <c r="E70" s="0">
         <v>0.00013607947353404726</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>1</v>
+        <v>4.3799999999999999</v>
       </c>
       <c r="B71" s="0">
         <v>1</v>
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="0">
-        <v>0.063463215198755238</v>
+        <v>1</v>
       </c>
       <c r="E71" s="0">
         <v>0.00010706671598718826</v>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B72" s="0">
         <v>1</v>
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="0">
-        <v>0.087456790039156587</v>
+        <v>1</v>
       </c>
       <c r="E72" s="0">
         <v>0.00010161263710645811</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>1</v>
+        <v>4.4199999999999999</v>
       </c>
       <c r="B73" s="0">
         <v>1</v>
@@ -3078,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="0">
-        <v>0.087578631249216832</v>
+        <v>1</v>
       </c>
       <c r="E73" s="0">
         <v>0.0001017536848361542</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>1</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="B74" s="0">
         <v>1</v>
@@ -3119,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="0">
-        <v>0.087583511308692283</v>
+        <v>1</v>
       </c>
       <c r="E74" s="0">
         <v>0.00010174094559310733</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>1</v>
+        <v>4.46</v>
       </c>
       <c r="B75" s="0">
         <v>1</v>
@@ -3160,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="0">
-        <v>0.087588160503437165</v>
+        <v>1</v>
       </c>
       <c r="E75" s="0">
         <v>0.00010171209165631831</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>1</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="B76" s="0">
         <v>1</v>
@@ -3201,7 +3201,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="0">
-        <v>0.088102509179220953</v>
+        <v>1</v>
       </c>
       <c r="E76" s="0">
         <v>0.00010300971580823293</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="B77" s="0">
         <v>1</v>
@@ -3242,7 +3242,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="0">
-        <v>0.08811299013398452</v>
+        <v>1</v>
       </c>
       <c r="E77" s="0">
         <v>0.0001030113486423037</v>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>1</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="B78" s="0">
         <v>1</v>
@@ -3283,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="D78" s="0">
-        <v>0.088122802382875412</v>
+        <v>1</v>
       </c>
       <c r="E78" s="0">
         <v>0.00010299340356197344</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>1</v>
+        <v>4.54</v>
       </c>
       <c r="B79" s="0">
         <v>1</v>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="0">
-        <v>0.075978945669713249</v>
+        <v>1</v>
       </c>
       <c r="E79" s="0">
         <v>0.00013560622999368629</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>1</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="B80" s="0">
         <v>1</v>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="D80" s="0">
-        <v>0.088142960976008683</v>
+        <v>1</v>
       </c>
       <c r="E80" s="0">
         <v>0.00010296484063562228</v>
@@ -3397,7 +3397,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>1</v>
+        <v>4.5800000000000001</v>
       </c>
       <c r="B81" s="0">
         <v>1</v>
@@ -3406,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="D81" s="0">
-        <v>0.052148984533024342</v>
+        <v>1</v>
       </c>
       <c r="E81" s="0">
         <v>0.00012974494931240914</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>1</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B82" s="0">
         <v>1</v>
@@ -3447,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="0">
-        <v>0.08757426264820499</v>
+        <v>1</v>
       </c>
       <c r="E82" s="0">
         <v>0.00010116338186759726</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>1</v>
+        <v>4.6200000000000001</v>
       </c>
       <c r="B83" s="0">
         <v>1</v>
@@ -3488,7 +3488,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="0">
-        <v>0.075963962129163454</v>
+        <v>1</v>
       </c>
       <c r="E83" s="0">
         <v>0.00013030100868227694</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>1</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="B84" s="0">
         <v>1</v>
@@ -3529,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="D84" s="0">
-        <v>0.087880394784640964</v>
+        <v>1</v>
       </c>
       <c r="E84" s="0">
         <v>0.00010176052752772182</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>1</v>
+        <v>4.6600000000000001</v>
       </c>
       <c r="B85" s="0">
         <v>1</v>
@@ -3570,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="0">
-        <v>0.052158451899895222</v>
+        <v>1</v>
       </c>
       <c r="E85" s="0">
         <v>0.00012745415046590849</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>1</v>
+        <v>4.6799999999999997</v>
       </c>
       <c r="B86" s="0">
         <v>1</v>
@@ -3611,7 +3611,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="0">
-        <v>0.052154573095297876</v>
+        <v>1</v>
       </c>
       <c r="E86" s="0">
         <v>0.00012801281159985286</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>1</v>
+        <v>4.7000000000000002</v>
       </c>
       <c r="B87" s="0">
         <v>1</v>
@@ -3652,7 +3652,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="0">
-        <v>0.052139763614268947</v>
+        <v>1</v>
       </c>
       <c r="E87" s="0">
         <v>0.00012533727442994949</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>1</v>
+        <v>4.7199999999999998</v>
       </c>
       <c r="B88" s="0">
         <v>1</v>
@@ -3693,7 +3693,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="0">
-        <v>0.087592885055525371</v>
+        <v>1</v>
       </c>
       <c r="E88" s="0">
         <v>0.00010055298954711705</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>1</v>
+        <v>4.7400000000000002</v>
       </c>
       <c r="B89" s="0">
         <v>1</v>
@@ -3734,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="D89" s="0">
-        <v>0.087590827027535817</v>
+        <v>1</v>
       </c>
       <c r="E89" s="0">
         <v>0.00010081447286221465</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>1</v>
+        <v>4.7599999999999998</v>
       </c>
       <c r="B90" s="0">
         <v>1</v>
@@ -3775,7 +3775,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="0">
-        <v>0.07561415955707447</v>
+        <v>1</v>
       </c>
       <c r="E90" s="0">
         <v>0.00012670342066962932</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>1</v>
+        <v>4.7800000000000002</v>
       </c>
       <c r="B91" s="0">
         <v>1</v>
@@ -3816,7 +3816,7 @@
         <v>1</v>
       </c>
       <c r="D91" s="0">
-        <v>0.087687749639841245</v>
+        <v>1</v>
       </c>
       <c r="E91" s="0">
         <v>0.0001004975440232535</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>1</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="B92" s="0">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="0">
-        <v>0.087729808419893182</v>
+        <v>1</v>
       </c>
       <c r="E92" s="0">
         <v>0.00010119837449476689</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>1</v>
+        <v>4.8200000000000003</v>
       </c>
       <c r="B93" s="0">
         <v>1</v>
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="D93" s="0">
-        <v>0.087821386225285097</v>
+        <v>1</v>
       </c>
       <c r="E93" s="0">
         <v>0.00010198529986716805</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>1</v>
+        <v>4.8399999999999999</v>
       </c>
       <c r="B94" s="0">
         <v>1</v>
@@ -3939,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="D94" s="0">
-        <v>0.087709790111383787</v>
+        <v>1</v>
       </c>
       <c r="E94" s="0">
         <v>0.00010094376588237815</v>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>1</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="B95" s="0">
         <v>1</v>
@@ -3980,7 +3980,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="0">
-        <v>0.087679225990227594</v>
+        <v>1</v>
       </c>
       <c r="E95" s="0">
         <v>0.0001021941200404179</v>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>1</v>
+        <v>4.8799999999999999</v>
       </c>
       <c r="B96" s="0">
         <v>1</v>
@@ -4021,7 +4021,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="0">
-        <v>0.08786451960364855</v>
+        <v>1</v>
       </c>
       <c r="E96" s="0">
         <v>0.00010001368577759336</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B97" s="0">
         <v>1</v>
@@ -4062,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="0">
-        <v>0.087748389668041521</v>
+        <v>1</v>
       </c>
       <c r="E97" s="0">
         <v>0.00010100254822539731</v>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>1</v>
+        <v>4.9199999999999999</v>
       </c>
       <c r="B98" s="0">
         <v>1</v>
@@ -4103,7 +4103,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="0">
-        <v>0.087501679738052784</v>
+        <v>1</v>
       </c>
       <c r="E98" s="0">
         <v>0.0001011946711444204</v>
@@ -4135,7 +4135,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>1</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="B99" s="0">
         <v>1</v>
@@ -4144,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="0">
-        <v>0.08766944611468519</v>
+        <v>1</v>
       </c>
       <c r="E99" s="0">
         <v>9.9872054452419443e-05</v>
@@ -4176,7 +4176,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>1</v>
+        <v>4.96</v>
       </c>
       <c r="B100" s="0">
         <v>1</v>
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
       <c r="D100" s="0">
-        <v>0.087748536768369204</v>
+        <v>1</v>
       </c>
       <c r="E100" s="0">
         <v>0.00010192522489863205</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>1</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="B101" s="0">
         <v>1</v>
@@ -4226,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="0">
-        <v>0.087760427768683369</v>
+        <v>1</v>
       </c>
       <c r="E101" s="0">
         <v>0.00010195846935724342</v>
@@ -4258,7 +4258,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B102" s="0">
         <v>1</v>
@@ -4267,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="0">
-        <v>0.087765961947604179</v>
+        <v>1</v>
       </c>
       <c r="E102" s="0">
         <v>0.00010181797320864355</v>
@@ -4299,7 +4299,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>1</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="B103" s="0">
         <v>1</v>
@@ -4308,7 +4308,7 @@
         <v>1</v>
       </c>
       <c r="D103" s="0">
-        <v>0.063625739135892367</v>
+        <v>1</v>
       </c>
       <c r="E103" s="0">
         <v>0.00010798174039716157</v>

</xml_diff>

<commit_message>
Push of any miscellaneous comments made on respective class or script
</commit_message>
<xml_diff>
--- a/Automation/Parsing/InterpolatedResults.xlsx
+++ b/Automation/Parsing/InterpolatedResults.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="72" uniqueCount="8">
   <si>
     <t>Strain 1 (in/in)</t>
   </si>
@@ -126,25 +126,25 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>8.9242944304159468e-05</v>
+        <v>8.9233778198276792e-05</v>
       </c>
       <c r="B2" s="0">
-        <v>5.7434759237437418e-05</v>
+        <v>5.7422936513186668e-05</v>
       </c>
       <c r="C2" s="0">
-        <v>4.7156680120753099e-05</v>
+        <v>4.7179169975268151e-05</v>
       </c>
       <c r="D2" s="0">
-        <v>4.241057476896423e-05</v>
+        <v>4.2393347700760489e-05</v>
       </c>
       <c r="E2" s="0">
-        <v>1.8410720166328673e-05</v>
+        <v>1.8435834717972008e-05</v>
       </c>
       <c r="F2" s="0">
-        <v>1.1909926190395775e-05</v>
+        <v>1.1927528123501968e-05</v>
       </c>
       <c r="G2" s="0">
-        <v>2.7240892790752301e-06</v>
+        <v>2.7214094798463219e-06</v>
       </c>
       <c r="H2" s="0">
         <v>2</v>
@@ -810,7 +810,9 @@
       <c r="C28" s="0">
         <v>4.7109409951152146e-05</v>
       </c>
-      <c r="D28" s="0"/>
+      <c r="D28" s="0">
+        <v>4.9789000000000001e-05</v>
+      </c>
       <c r="E28" s="0">
         <v>1.7188640238708385e-05</v>
       </c>
@@ -2859,7 +2861,9 @@
       <c r="B107" s="0">
         <v>7.1948937913065257e-05</v>
       </c>
-      <c r="C107" s="0"/>
+      <c r="C107" s="0">
+        <v>6.3816e-05</v>
+      </c>
       <c r="D107" s="0">
         <v>3.7326166305992132e-05</v>
       </c>
@@ -4151,7 +4155,9 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="0"/>
+      <c r="A157" s="0">
+        <v>3.9736e-05</v>
+      </c>
       <c r="B157" s="0">
         <v>5.0121281207758925e-05</v>
       </c>

</xml_diff>

<commit_message>
New strain study values and associated CSVs
</commit_message>
<xml_diff>
--- a/Automation/Parsing/InterpolatedResults.xlsx
+++ b/Automation/Parsing/InterpolatedResults.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="88" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="136" uniqueCount="8">
   <si>
     <t>Strain 1 (in/in)</t>
   </si>
@@ -89,11 +89,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5546875" customWidth="true"/>
-    <col min="2" max="2" width="15.21875" customWidth="true"/>
-    <col min="3" max="3" width="15.21875" customWidth="true"/>
-    <col min="4" max="4" width="15.21875" customWidth="true"/>
-    <col min="5" max="5" width="15.21875" customWidth="true"/>
-    <col min="6" max="6" width="15.21875" customWidth="true"/>
+    <col min="2" max="2" width="15.5546875" customWidth="true"/>
+    <col min="3" max="3" width="15.5546875" customWidth="true"/>
+    <col min="4" max="4" width="15.5546875" customWidth="true"/>
+    <col min="5" max="5" width="15.5546875" customWidth="true"/>
+    <col min="6" max="6" width="15.5546875" customWidth="true"/>
     <col min="7" max="7" width="15.21875" customWidth="true"/>
     <col min="8" max="8" width="10.88671875" customWidth="true"/>
   </cols>
@@ -126,132 +126,132 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>8.9233778198276792e-05</v>
+        <v>0.00038182392884372258</v>
       </c>
       <c r="B2" s="0">
-        <v>5.7422936513186668e-05</v>
+        <v>0.00035403039842678725</v>
       </c>
       <c r="C2" s="0">
-        <v>4.7179169975268151e-05</v>
+        <v>0.00029786839697544439</v>
       </c>
       <c r="D2" s="0">
-        <v>4.2393347700760489e-05</v>
+        <v>0.00028047487531956641</v>
       </c>
       <c r="E2" s="0">
-        <v>1.8435834717972008e-05</v>
+        <v>0.00015149541401110123</v>
       </c>
       <c r="F2" s="0">
-        <v>1.1927528123501968e-05</v>
+        <v>7.3537178411631562e-05</v>
       </c>
       <c r="G2" s="0">
-        <v>2.7214094798463219e-06</v>
+        <v>4.7948218254677212e-05</v>
       </c>
       <c r="H2" s="0">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>9.4161775578972256e-05</v>
+        <v>0.00042263658554286913</v>
       </c>
       <c r="B3" s="0">
-        <v>6.4866357860474339e-05</v>
+        <v>0.00039022460742583592</v>
       </c>
       <c r="C3" s="0">
-        <v>4.5568745247885025e-05</v>
+        <v>0.0002824991476365973</v>
       </c>
       <c r="D3" s="0">
-        <v>3.6706211577229814e-05</v>
+        <v>0.00025123454853737641</v>
       </c>
       <c r="E3" s="0">
-        <v>1.9494312099251218e-05</v>
+        <v>0.00015649654231147101</v>
       </c>
       <c r="F3" s="0">
-        <v>1.2434002509512417e-05</v>
+        <v>8.6109326009228211e-05</v>
       </c>
       <c r="G3" s="0">
-        <v>2.9845036399297476e-06</v>
+        <v>4.4668336411425145e-05</v>
       </c>
       <c r="H3" s="0">
-        <v>2.02</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.00010003253440793698</v>
+        <v>0.00038507274854935063</v>
       </c>
       <c r="B4" s="0">
-        <v>8.3433528507576867e-05</v>
+        <v>0.00036483926768487594</v>
       </c>
       <c r="C4" s="0">
-        <v>6.5768198884758202e-05</v>
+        <v>0.00031992875715390091</v>
       </c>
       <c r="D4" s="0">
-        <v>4.855608160525657e-05</v>
+        <v>0.00026506155257288694</v>
       </c>
       <c r="E4" s="0">
-        <v>2.337922213575963e-05</v>
+        <v>0.0001591575848330936</v>
       </c>
       <c r="F4" s="0">
-        <v>1.4770337290020662e-05</v>
+        <v>9.78150678888276e-05</v>
       </c>
       <c r="G4" s="0">
-        <v>3.2019521984828219e-06</v>
+        <v>4.9136529576521611e-05</v>
       </c>
       <c r="H4" s="0">
-        <v>2.04</v>
+        <v>18.199999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>9.7712479179607142e-05</v>
+        <v>0.0004327808641336705</v>
       </c>
       <c r="B5" s="0">
-        <v>6.2403299283221922e-05</v>
+        <v>0.0003758961980946703</v>
       </c>
       <c r="C5" s="0">
-        <v>4.4962595871037605e-05</v>
+        <v>0.00028380656905634393</v>
       </c>
       <c r="D5" s="0">
-        <v>3.8374679927770257e-05</v>
+        <v>0.00026968978035771517</v>
       </c>
       <c r="E5" s="0">
-        <v>1.9168174461614287e-05</v>
+        <v>0.00015331144650088585</v>
       </c>
       <c r="F5" s="0">
-        <v>1.1254982424401248e-05</v>
+        <v>0.0001087361715420914</v>
       </c>
       <c r="G5" s="0">
-        <v>2.9905176540109287e-06</v>
+        <v>4.3458412126515643e-05</v>
       </c>
       <c r="H5" s="0">
-        <v>2.0600000000000001</v>
+        <v>18.300000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9.6859867596732943e-05</v>
+        <v>0.00038938738530532144</v>
       </c>
       <c r="B6" s="0">
-        <v>6.3075322769717016e-05</v>
+        <v>0.00037742531329545569</v>
       </c>
       <c r="C6" s="0">
-        <v>4.4732136143123262e-05</v>
+        <v>0.00036146000000000003</v>
       </c>
       <c r="D6" s="0">
-        <v>3.8871977402178555e-05</v>
+        <v>0.00025353881884849821</v>
       </c>
       <c r="E6" s="0">
-        <v>1.9004261447992196e-05</v>
+        <v>0.000169765067159418</v>
       </c>
       <c r="F6" s="0">
-        <v>1.0869073004057195e-05</v>
+        <v>9.6568531907344939e-05</v>
       </c>
       <c r="G6" s="0">
-        <v>2.9959360747522298e-06</v>
+        <v>5.1150164233478986e-05</v>
       </c>
       <c r="H6" s="0">
-        <v>2.0800000000000001</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="7">

</xml_diff>